<commit_message>
Lab Routers semana 13
</commit_message>
<xml_diff>
--- a/Proyecto Redes 2/AnalisisSistemaRed.xlsx
+++ b/Proyecto Redes 2/AnalisisSistemaRed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/916453d256f63eb8/Documentos/GitHub/CursosRedes/Proyecto Redes 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1112" documentId="11_AD4D2F04E46CFB4ACB3E20CB0D92F634683EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8268B346-BE39-43E4-BE5B-7E05690A2A3D}"/>
+  <xr:revisionPtr revIDLastSave="1116" documentId="11_AD4D2F04E46CFB4ACB3E20CB0D92F634683EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D8E9E2F-853E-4418-8E88-6C8D606C36F8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30675" yWindow="1875" windowWidth="28800" windowHeight="15285" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dispositivos Necesarios" sheetId="1" r:id="rId1"/>
@@ -937,7 +937,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -995,6 +995,14 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1025,15 +1033,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -1321,7 +1320,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H4" sqref="H4:H9"/>
     </sheetView>
   </sheetViews>
@@ -1677,15 +1676,15 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21">
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25">
         <v>6</v>
       </c>
-      <c r="G20" s="21"/>
+      <c r="G20" s="25"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C13:F18">
@@ -1703,8 +1702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2EF6F0D-2255-4E4A-984B-81F981B54FDE}">
   <dimension ref="B2:M28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1738,14 +1737,14 @@
       </c>
     </row>
     <row r="3" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
     </row>
     <row r="4" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
@@ -1831,19 +1830,19 @@
         <v>28</v>
       </c>
       <c r="J6">
-        <v>500</v>
+        <v>80</v>
       </c>
       <c r="K6">
         <f>J6*50</f>
-        <v>25000</v>
+        <v>4000</v>
       </c>
       <c r="L6">
         <f>J6*10</f>
-        <v>5000</v>
+        <v>800</v>
       </c>
       <c r="M6">
         <f>SUM(K6:L6)</f>
-        <v>30000</v>
+        <v>4800</v>
       </c>
     </row>
     <row r="7" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
@@ -1910,16 +1909,16 @@
       </c>
     </row>
     <row r="10" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-    </row>
-    <row r="11" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+    </row>
+    <row r="11" spans="2:13" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>45</v>
       </c>
@@ -2025,20 +2024,20 @@
       </c>
     </row>
     <row r="16" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
     </row>
     <row r="17" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="25"/>
+      <c r="C17" s="29"/>
       <c r="D17" s="4">
         <v>1</v>
       </c>
@@ -2054,10 +2053,10 @@
       </c>
     </row>
     <row r="18" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="25"/>
+      <c r="C18" s="29"/>
       <c r="D18" s="4">
         <v>1</v>
       </c>
@@ -2073,12 +2072,12 @@
       </c>
     </row>
     <row r="19" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
       <c r="F19" s="10">
         <f>SUM(F4:F9,F11:F15,F17:F18)</f>
         <v>69569.45</v>
@@ -2209,7 +2208,7 @@
       </c>
     </row>
     <row r="4" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="33" t="s">
         <v>77</v>
       </c>
       <c r="C4" s="12" t="s">
@@ -2223,7 +2222,7 @@
       </c>
     </row>
     <row r="5" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="29"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="12" t="s">
         <v>61</v>
       </c>
@@ -2235,7 +2234,7 @@
       </c>
     </row>
     <row r="6" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="29"/>
+      <c r="B6" s="33"/>
       <c r="C6" s="12" t="s">
         <v>62</v>
       </c>
@@ -2247,7 +2246,7 @@
       </c>
     </row>
     <row r="7" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="34" t="s">
         <v>78</v>
       </c>
       <c r="C7" s="12" t="s">
@@ -2261,7 +2260,7 @@
       </c>
     </row>
     <row r="8" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="30"/>
+      <c r="B8" s="34"/>
       <c r="C8" s="12" t="s">
         <v>64</v>
       </c>
@@ -2273,7 +2272,7 @@
       </c>
     </row>
     <row r="9" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="34" t="s">
         <v>79</v>
       </c>
       <c r="C9" s="12" t="s">
@@ -2287,7 +2286,7 @@
       </c>
     </row>
     <row r="10" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="30"/>
+      <c r="B10" s="34"/>
       <c r="C10" s="12" t="s">
         <v>66</v>
       </c>
@@ -2299,7 +2298,7 @@
       </c>
     </row>
     <row r="11" spans="2:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="B11" s="30"/>
+      <c r="B11" s="34"/>
       <c r="C11" s="3" t="s">
         <v>67</v>
       </c>
@@ -2311,7 +2310,7 @@
       </c>
     </row>
     <row r="12" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="34" t="s">
         <v>80</v>
       </c>
       <c r="C12" s="12" t="s">
@@ -2325,7 +2324,7 @@
       </c>
     </row>
     <row r="13" spans="2:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="B13" s="30"/>
+      <c r="B13" s="34"/>
       <c r="C13" s="3" t="s">
         <v>69</v>
       </c>
@@ -2337,7 +2336,7 @@
       </c>
     </row>
     <row r="14" spans="2:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="B14" s="30"/>
+      <c r="B14" s="34"/>
       <c r="C14" s="3" t="s">
         <v>70</v>
       </c>
@@ -2349,7 +2348,7 @@
       </c>
     </row>
     <row r="15" spans="2:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="34" t="s">
         <v>81</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -2363,7 +2362,7 @@
       </c>
     </row>
     <row r="16" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B16" s="30"/>
+      <c r="B16" s="34"/>
       <c r="C16" s="12" t="s">
         <v>72</v>
       </c>
@@ -2375,7 +2374,7 @@
       </c>
     </row>
     <row r="17" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B17" s="30"/>
+      <c r="B17" s="34"/>
       <c r="C17" s="12" t="s">
         <v>73</v>
       </c>
@@ -2387,7 +2386,7 @@
       </c>
     </row>
     <row r="18" spans="2:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="34" t="s">
         <v>82</v>
       </c>
       <c r="C18" s="12" t="s">
@@ -2401,7 +2400,7 @@
       </c>
     </row>
     <row r="19" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B19" s="30"/>
+      <c r="B19" s="34"/>
       <c r="C19" s="12" t="s">
         <v>75</v>
       </c>
@@ -2413,14 +2412,14 @@
       </c>
     </row>
     <row r="20" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="C20" s="27"/>
-      <c r="D20" s="28" t="s">
+      <c r="C20" s="31"/>
+      <c r="D20" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="E20" s="28"/>
+      <c r="E20" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2455,39 +2454,39 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="23" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="21" t="s">
         <v>251</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="G4" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="H4" s="32" t="s">
+      <c r="H4" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="I4" s="32" t="s">
+      <c r="I4" s="22" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2498,22 +2497,22 @@
       <c r="C5" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="E5" s="34" t="s">
+      <c r="E5" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="F5" s="34" t="s">
+      <c r="F5" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="G5" s="34" t="s">
+      <c r="G5" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="H5" s="34" t="s">
+      <c r="H5" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="I5" s="34" t="s">
+      <c r="I5" s="24" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2524,22 +2523,22 @@
       <c r="C6" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="E6" s="34" t="s">
+      <c r="E6" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="F6" s="34" t="s">
+      <c r="F6" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="G6" s="34" t="s">
+      <c r="G6" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="H6" s="34" t="s">
+      <c r="H6" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="I6" s="34" t="s">
+      <c r="I6" s="24" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2550,22 +2549,22 @@
       <c r="C7" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="E7" s="34" t="s">
+      <c r="E7" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="F7" s="34" t="s">
+      <c r="F7" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="G7" s="34" t="s">
+      <c r="G7" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="H7" s="34" t="s">
+      <c r="H7" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="I7" s="34" t="s">
+      <c r="I7" s="24" t="s">
         <v>145</v>
       </c>
     </row>
@@ -2576,22 +2575,22 @@
       <c r="C8" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="E8" s="34" t="s">
+      <c r="E8" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="F8" s="34" t="s">
+      <c r="F8" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="G8" s="34" t="s">
+      <c r="G8" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="H8" s="34" t="s">
+      <c r="H8" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="I8" s="34" t="s">
+      <c r="I8" s="24" t="s">
         <v>149</v>
       </c>
     </row>
@@ -2602,22 +2601,22 @@
       <c r="C9" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="D9" s="34" t="s">
+      <c r="D9" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="E9" s="34" t="s">
+      <c r="E9" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="F9" s="34" t="s">
+      <c r="F9" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="G9" s="34" t="s">
+      <c r="G9" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="H9" s="34" t="s">
+      <c r="H9" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="I9" s="34" t="s">
+      <c r="I9" s="24" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2628,22 +2627,22 @@
       <c r="C10" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="E10" s="34" t="s">
+      <c r="E10" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="F10" s="34" t="s">
+      <c r="F10" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G10" s="34" t="s">
+      <c r="G10" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="H10" s="34" t="s">
+      <c r="H10" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="I10" s="34" t="s">
+      <c r="I10" s="24" t="s">
         <v>157</v>
       </c>
     </row>
@@ -2654,22 +2653,22 @@
       <c r="C11" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="D11" s="34" t="s">
+      <c r="D11" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="E11" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="F11" s="34" t="s">
+      <c r="F11" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="G11" s="35" t="s">
+      <c r="G11" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="H11" s="35" t="s">
+      <c r="H11" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="I11" s="34" t="s">
+      <c r="I11" s="24" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2680,22 +2679,22 @@
       <c r="C12" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D12" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="E12" s="34" t="s">
+      <c r="E12" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="F12" s="34" t="s">
+      <c r="F12" s="24" t="s">
         <v>179</v>
       </c>
-      <c r="G12" s="34" t="s">
+      <c r="G12" s="24" t="s">
         <v>206</v>
       </c>
-      <c r="H12" s="34" t="s">
+      <c r="H12" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="I12" s="34" t="s">
+      <c r="I12" s="24" t="s">
         <v>180</v>
       </c>
     </row>
@@ -2706,22 +2705,22 @@
       <c r="C13" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="D13" s="34" t="s">
+      <c r="D13" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="E13" s="34" t="s">
+      <c r="E13" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="F13" s="34" t="s">
+      <c r="F13" s="24" t="s">
         <v>183</v>
       </c>
-      <c r="G13" s="34" t="s">
+      <c r="G13" s="24" t="s">
         <v>207</v>
       </c>
-      <c r="H13" s="34" t="s">
+      <c r="H13" s="24" t="s">
         <v>181</v>
       </c>
-      <c r="I13" s="34" t="s">
+      <c r="I13" s="24" t="s">
         <v>182</v>
       </c>
     </row>
@@ -2732,22 +2731,22 @@
       <c r="C14" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="D14" s="34" t="s">
+      <c r="D14" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="E14" s="34" t="s">
+      <c r="E14" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="F14" s="34" t="s">
+      <c r="F14" s="24" t="s">
         <v>184</v>
       </c>
-      <c r="G14" s="34" t="s">
+      <c r="G14" s="24" t="s">
         <v>208</v>
       </c>
-      <c r="H14" s="34" t="s">
+      <c r="H14" s="24" t="s">
         <v>218</v>
       </c>
-      <c r="I14" s="34" t="s">
+      <c r="I14" s="24" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2758,22 +2757,22 @@
       <c r="C15" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D15" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="E15" s="34" t="s">
+      <c r="E15" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="F15" s="34" t="s">
+      <c r="F15" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="G15" s="34" t="s">
+      <c r="G15" s="24" t="s">
         <v>209</v>
       </c>
-      <c r="H15" s="34" t="s">
+      <c r="H15" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="I15" s="34" t="s">
+      <c r="I15" s="24" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2784,22 +2783,22 @@
       <c r="C16" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="D16" s="34" t="s">
+      <c r="D16" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="E16" s="34" t="s">
+      <c r="E16" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="F16" s="34" t="s">
+      <c r="F16" s="24" t="s">
         <v>188</v>
       </c>
-      <c r="G16" s="34" t="s">
+      <c r="G16" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="H16" s="34" t="s">
+      <c r="H16" s="24" t="s">
         <v>187</v>
       </c>
-      <c r="I16" s="34" t="s">
+      <c r="I16" s="24" t="s">
         <v>189</v>
       </c>
     </row>
@@ -2810,22 +2809,22 @@
       <c r="C17" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="D17" s="34" t="s">
+      <c r="D17" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="E17" s="34" t="s">
+      <c r="E17" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="F17" s="34" t="s">
+      <c r="F17" s="24" t="s">
         <v>190</v>
       </c>
-      <c r="G17" s="34" t="s">
+      <c r="G17" s="24" t="s">
         <v>211</v>
       </c>
-      <c r="H17" s="34" t="s">
+      <c r="H17" s="24" t="s">
         <v>220</v>
       </c>
-      <c r="I17" s="34" t="s">
+      <c r="I17" s="24" t="s">
         <v>191</v>
       </c>
     </row>
@@ -2836,22 +2835,22 @@
       <c r="C18" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="D18" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="E18" s="34" t="s">
+      <c r="E18" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="F18" s="34" t="s">
+      <c r="F18" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="G18" s="34" t="s">
+      <c r="G18" s="24" t="s">
         <v>212</v>
       </c>
-      <c r="H18" s="34" t="s">
+      <c r="H18" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="I18" s="34" t="s">
+      <c r="I18" s="24" t="s">
         <v>193</v>
       </c>
     </row>
@@ -2862,22 +2861,22 @@
       <c r="C19" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="D19" s="34" t="s">
+      <c r="D19" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="E19" s="34" t="s">
+      <c r="E19" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="F19" s="34" t="s">
+      <c r="F19" s="24" t="s">
         <v>194</v>
       </c>
-      <c r="G19" s="34" t="s">
+      <c r="G19" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="24" t="s">
         <v>222</v>
       </c>
-      <c r="I19" s="34" t="s">
+      <c r="I19" s="24" t="s">
         <v>195</v>
       </c>
     </row>
@@ -2888,22 +2887,22 @@
       <c r="C20" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="D20" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="E20" s="34" t="s">
+      <c r="E20" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="F20" s="34" t="s">
+      <c r="F20" s="24" t="s">
         <v>196</v>
       </c>
-      <c r="G20" s="34" t="s">
+      <c r="G20" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="H20" s="34" t="s">
+      <c r="H20" s="24" t="s">
         <v>198</v>
       </c>
-      <c r="I20" s="34" t="s">
+      <c r="I20" s="24" t="s">
         <v>199</v>
       </c>
     </row>
@@ -2914,22 +2913,22 @@
       <c r="C21" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="D21" s="34" t="s">
+      <c r="D21" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="E21" s="34" t="s">
+      <c r="E21" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="F21" s="34" t="s">
+      <c r="F21" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="G21" s="34" t="s">
+      <c r="G21" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="H21" s="34" t="s">
+      <c r="H21" s="24" t="s">
         <v>223</v>
       </c>
-      <c r="I21" s="34" t="s">
+      <c r="I21" s="24" t="s">
         <v>201</v>
       </c>
     </row>
@@ -2940,22 +2939,22 @@
       <c r="C22" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="D22" s="34" t="s">
+      <c r="D22" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="E22" s="34" t="s">
+      <c r="E22" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="F22" s="34" t="s">
+      <c r="F22" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="G22" s="34" t="s">
+      <c r="G22" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="H22" s="34" t="s">
+      <c r="H22" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="I22" s="34" t="s">
+      <c r="I22" s="24" t="s">
         <v>203</v>
       </c>
     </row>
@@ -2966,22 +2965,22 @@
       <c r="C23" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="D23" s="34" t="s">
+      <c r="D23" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="E23" s="34" t="s">
+      <c r="E23" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="F23" s="34" t="s">
+      <c r="F23" s="24" t="s">
         <v>204</v>
       </c>
-      <c r="G23" s="34" t="s">
+      <c r="G23" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="H23" s="34" t="s">
+      <c r="H23" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="I23" s="34" t="s">
+      <c r="I23" s="24" t="s">
         <v>205</v>
       </c>
     </row>
@@ -2992,22 +2991,22 @@
       <c r="C24" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="34" t="s">
+      <c r="D24" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="E24" s="34" t="s">
+      <c r="E24" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="F24" s="34" t="s">
+      <c r="F24" s="24" t="s">
         <v>231</v>
       </c>
-      <c r="G24" s="34" t="s">
+      <c r="G24" s="24" t="s">
         <v>232</v>
       </c>
-      <c r="H24" s="34" t="s">
+      <c r="H24" s="24" t="s">
         <v>233</v>
       </c>
-      <c r="I24" s="34" t="s">
+      <c r="I24" s="24" t="s">
         <v>234</v>
       </c>
     </row>
@@ -3018,22 +3017,22 @@
       <c r="C25" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="D25" s="34" t="s">
+      <c r="D25" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="E25" s="34" t="s">
+      <c r="E25" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="F25" s="34" t="s">
+      <c r="F25" s="24" t="s">
         <v>235</v>
       </c>
-      <c r="G25" s="34" t="s">
+      <c r="G25" s="24" t="s">
         <v>236</v>
       </c>
-      <c r="H25" s="34" t="s">
+      <c r="H25" s="24" t="s">
         <v>237</v>
       </c>
-      <c r="I25" s="34" t="s">
+      <c r="I25" s="24" t="s">
         <v>238</v>
       </c>
     </row>
@@ -3044,22 +3043,22 @@
       <c r="C26" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="D26" s="34" t="s">
+      <c r="D26" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="E26" s="34" t="s">
+      <c r="E26" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="F26" s="34" t="s">
+      <c r="F26" s="24" t="s">
         <v>239</v>
       </c>
-      <c r="G26" s="34" t="s">
+      <c r="G26" s="24" t="s">
         <v>240</v>
       </c>
-      <c r="H26" s="34" t="s">
+      <c r="H26" s="24" t="s">
         <v>241</v>
       </c>
-      <c r="I26" s="34" t="s">
+      <c r="I26" s="24" t="s">
         <v>242</v>
       </c>
     </row>
@@ -3070,22 +3069,22 @@
       <c r="C27" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="D27" s="34" t="s">
+      <c r="D27" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="E27" s="34" t="s">
+      <c r="E27" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="F27" s="34" t="s">
+      <c r="F27" s="24" t="s">
         <v>243</v>
       </c>
-      <c r="G27" s="34" t="s">
+      <c r="G27" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="H27" s="34" t="s">
+      <c r="H27" s="24" t="s">
         <v>245</v>
       </c>
-      <c r="I27" s="34" t="s">
+      <c r="I27" s="24" t="s">
         <v>246</v>
       </c>
     </row>
@@ -3096,22 +3095,22 @@
       <c r="C28" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="D28" s="34" t="s">
+      <c r="D28" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="E28" s="34" t="s">
+      <c r="E28" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="F28" s="34" t="s">
+      <c r="F28" s="24" t="s">
         <v>247</v>
       </c>
-      <c r="G28" s="34" t="s">
+      <c r="G28" s="24" t="s">
         <v>248</v>
       </c>
-      <c r="H28" s="34" t="s">
+      <c r="H28" s="24" t="s">
         <v>249</v>
       </c>
-      <c r="I28" s="34" t="s">
+      <c r="I28" s="24" t="s">
         <v>250</v>
       </c>
     </row>

</xml_diff>